<commit_message>
Added unit test code
Added unit test code, made lots of changes to namespaces, added a
run_all routine and code for R for unit testing. Lots of progress but
many more tests to add.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7160" yWindow="0" windowWidth="18480" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11380" yWindow="0" windowWidth="14260" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="242">
   <si>
     <t>Test</t>
   </si>
@@ -635,6 +635,117 @@
   </si>
   <si>
     <t>0.4600, 1.6270, 13.9785,18.5090,19.0210</t>
+  </si>
+  <si>
+    <t>Q1 0.25</t>
+  </si>
+  <si>
+    <t>longvec</t>
+  </si>
+  <si>
+    <t>Q1 0.75</t>
+  </si>
+  <si>
+    <t>Q2 0.25</t>
+  </si>
+  <si>
+    <t>Q2 0.75</t>
+  </si>
+  <si>
+    <t>Q3 0.25</t>
+  </si>
+  <si>
+    <t>Q4 0.75</t>
+  </si>
+  <si>
+    <t>Q3 0.75</t>
+  </si>
+  <si>
+    <t>Q4 0.25</t>
+  </si>
+  <si>
+    <t>Q5 0.25</t>
+  </si>
+  <si>
+    <t>Q5 0.75</t>
+  </si>
+  <si>
+    <t>Q6 0.25</t>
+  </si>
+  <si>
+    <t>Q6 0.75</t>
+  </si>
+  <si>
+    <t>Q7 0.25</t>
+  </si>
+  <si>
+    <t>Q7 0.75</t>
+  </si>
+  <si>
+    <t>Q8 0.25</t>
+  </si>
+  <si>
+    <t>Q8 0.75</t>
+  </si>
+  <si>
+    <t>Q9 0.25</t>
+  </si>
+  <si>
+    <t>Q9 0.75</t>
+  </si>
+  <si>
+    <t>2.889</t>
+  </si>
+  <si>
+    <t>3.1175</t>
+  </si>
+  <si>
+    <t>3.00325</t>
+  </si>
+  <si>
+    <t>3.23175</t>
+  </si>
+  <si>
+    <t>3.079417</t>
+  </si>
+  <si>
+    <t>3.088938</t>
+  </si>
+  <si>
+    <t>7.462</t>
+  </si>
+  <si>
+    <t>7.468</t>
+  </si>
+  <si>
+    <t>7.102</t>
+  </si>
+  <si>
+    <t>7.678</t>
+  </si>
+  <si>
+    <t>7.39</t>
+  </si>
+  <si>
+    <t>6.814</t>
+  </si>
+  <si>
+    <t>7.486</t>
+  </si>
+  <si>
+    <t>Stderror</t>
+  </si>
+  <si>
+    <t>2.887254</t>
+  </si>
+  <si>
+    <t>3.402884</t>
+  </si>
+  <si>
+    <t>FAILED!</t>
+  </si>
+  <si>
+    <t>4.406583</t>
   </si>
 </sst>
 </file>
@@ -698,8 +809,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="81">
+  <cellStyleXfs count="95">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -787,7 +912,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="81">
+  <cellStyles count="95">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -828,6 +953,13 @@
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -868,6 +1000,13 @@
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2305,18 +2444,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:E72"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" style="2" customWidth="1"/>
     <col min="3" max="4" width="25.1640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="32.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2695,7 +2834,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
         <v>183</v>
       </c>
@@ -2703,7 +2842,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
         <v>183</v>
       </c>
@@ -2714,7 +2853,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
         <v>183</v>
       </c>
@@ -2725,7 +2864,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
         <v>183</v>
       </c>
@@ -2733,7 +2872,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
         <v>190</v>
       </c>
@@ -2744,7 +2883,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
         <v>190</v>
       </c>
@@ -2755,7 +2894,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
         <v>190</v>
       </c>
@@ -2766,7 +2905,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
         <v>190</v>
       </c>
@@ -2777,7 +2916,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
         <v>190</v>
       </c>
@@ -2785,7 +2924,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
         <v>191</v>
       </c>
@@ -2796,7 +2935,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
         <v>191</v>
       </c>
@@ -2807,7 +2946,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
         <v>191</v>
       </c>
@@ -2818,7 +2957,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
         <v>191</v>
       </c>
@@ -2829,7 +2968,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
         <v>191</v>
       </c>
@@ -2837,56 +2976,413 @@
         <v>165</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3">
+        <v>238</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>194</v>
+        <v>159</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3">
+        <v>239</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
         <v>76</v>
       </c>
       <c r="B51" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B53" s="2" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Algorithm corrections, more unit tests
Added more unit tests and corrected some bugs in the Frequencies and
UniqueVals algorithms. Added a new variable for testing the
frequency-based algorithms.
</commit_message>
<xml_diff>
--- a/Progress.xlsx
+++ b/Progress.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22202"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11380" yWindow="0" windowWidth="14260" windowHeight="14560" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="15300" yWindow="0" windowWidth="10340" windowHeight="14560" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="249">
   <si>
     <t>Test</t>
   </si>
@@ -746,6 +746,27 @@
   </si>
   <si>
     <t>4.406583</t>
+  </si>
+  <si>
+    <t>range</t>
+  </si>
+  <si>
+    <t>18.561</t>
+  </si>
+  <si>
+    <t>UniqueVals</t>
+  </si>
+  <si>
+    <t>uniques</t>
+  </si>
+  <si>
+    <t>uniqmis</t>
+  </si>
+  <si>
+    <t>[1,2,3,4] [2,7,5,2]</t>
+  </si>
+  <si>
+    <t>[1,2,3,4] [2,7,3,1]</t>
   </si>
 </sst>
 </file>
@@ -809,8 +830,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="95">
+  <cellStyleXfs count="119">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -912,7 +957,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="95">
+  <cellStyles count="119">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -960,6 +1005,18 @@
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1007,6 +1064,18 @@
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2444,10 +2513,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E72"/>
+  <dimension ref="A1:E78"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2694,7 +2763,7 @@
         <v>158</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2749,7 +2818,7 @@
         <v>158</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2776,397 +2845,361 @@
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>153</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>182</v>
+        <v>242</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>159</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>182</v>
+        <v>244</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>165</v>
+        <v>245</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B38" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C38" s="2" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
-      <c r="A33" s="2" t="s">
+    <row r="39" spans="1:3">
+      <c r="A39" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
-      <c r="A34" s="2" t="s">
+    <row r="40" spans="1:3">
+      <c r="A40" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
-      <c r="A35" s="2" t="s">
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C41" s="2" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B42" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B43" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="C43" s="2" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
+    <row r="44" spans="1:3">
+      <c r="A44" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
+    <row r="45" spans="1:3">
+      <c r="A45" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B46" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C46" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
         <v>190</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B48" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>197</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>153</v>
+        <v>194</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>76</v>
+        <v>191</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>204</v>
+        <v>165</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>76</v>
+        <v>237</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>205</v>
+        <v>237</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>155</v>
+        <v>240</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>207</v>
+        <v>76</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>206</v>
+        <v>153</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>155</v>
+        <v>201</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>208</v>
+        <v>76</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>155</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>209</v>
+        <v>76</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>206</v>
+        <v>158</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>155</v>
+        <v>203</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>210</v>
+        <v>76</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>155</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>212</v>
+        <v>76</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>206</v>
@@ -3183,7 +3216,7 @@
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>206</v>
@@ -3200,7 +3233,7 @@
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>206</v>
@@ -3217,7 +3250,7 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>206</v>
@@ -3234,16 +3267,16 @@
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="E64" s="2" t="s">
         <v>155</v>
@@ -3251,16 +3284,16 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>155</v>
@@ -3268,16 +3301,16 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E66" s="2" t="s">
         <v>155</v>
@@ -3285,16 +3318,16 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>155</v>
@@ -3302,16 +3335,16 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>155</v>
@@ -3319,16 +3352,16 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>155</v>
@@ -3336,16 +3369,16 @@
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="E70" s="2" t="s">
         <v>155</v>
@@ -3353,16 +3386,16 @@
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="2" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E71" s="2" t="s">
         <v>155</v>
@@ -3370,18 +3403,120 @@
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="2" t="s">
-        <v>79</v>
+        <v>218</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>206</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C78" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D72" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="E72" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>